<commit_message>
Updated CanBusOff_swc.arxml Added HkmcDiag_swc.arxml Added HkmcDtc_swc.arxml
</commit_message>
<xml_diff>
--- a/R0/02_SignalMatrix/HkmcDiag/HkmcDiag_SignalMatrix_V1_R0.xlsx
+++ b/R0/02_SignalMatrix/HkmcDiag/HkmcDiag_SignalMatrix_V1_R0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\00_2020\90_GitHub\0410\Veoneer\R0\02_SignalMatrix\HkmcDiag\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7546EF5-4D59-4B44-B8A3-C6B854479827}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4572C7-D58F-41E7-A41B-E2EABB655042}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{51B81819-EC55-40BC-AC3D-96F7FA05F5FF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{51B81819-EC55-40BC-AC3D-96F7FA05F5FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="22" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>Change Log</t>
   </si>
@@ -142,28 +142,16 @@
     <t>C/S</t>
   </si>
   <si>
-    <t>Function Name/Signal Group</t>
-  </si>
-  <si>
     <t>Input Parameters</t>
   </si>
   <si>
     <t>Output Parameters</t>
   </si>
   <si>
-    <t>HkmcEolCodingRead</t>
-  </si>
-  <si>
-    <t>HkmcEolCodingWrite</t>
-  </si>
-  <si>
     <t>HkmcEolData</t>
   </si>
   <si>
     <t>WriteStatus</t>
-  </si>
-  <si>
-    <t>ReadStatus</t>
   </si>
   <si>
     <t>Description</t>
@@ -175,6 +163,24 @@
     <t xml:space="preserve">
 Struct HkmcEolData
 </t>
+  </si>
+  <si>
+    <t>ReadStatus: 
+0:  Failed
+1: Success</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bool
+</t>
+  </si>
+  <si>
+    <t>WriteStatus: 
+0:  Failed
+1: Success</t>
+  </si>
+  <si>
+    <t>HkmcEolCoding</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Sizeof(HkmcEolData) = 8B .
@@ -185,38 +191,58 @@
 U8 data5;U8 data6;
 U8 data7;U8 data8
 }</t>
-  </si>
-  <si>
-    <t>ReadStatus: 
-0:  Failed
-1: Success</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bool
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Struct HkmcEolData
 </t>
-  </si>
-  <si>
-    <t>WriteStatus: 
-0:  Failed
-1: Success</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>HkmcEolData</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HkmcEolCodingRead/HkmcEolCoding</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>HkmcEolCodingWrite/HkmcEolCoding</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Function Name/Signal Group</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ReadStatus</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>e.g.)HkmcEolCodingRead(in HkmcEolData,  out bool ReadStatus)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -227,7 +253,7 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -236,7 +262,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -244,20 +270,20 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -265,7 +291,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -273,7 +299,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -281,14 +307,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -809,6 +835,30 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -818,24 +868,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -847,12 +879,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -871,7 +897,7 @@
     <cellStyle name="Normal 7" xfId="11" xr:uid="{39D77901-4BCA-40AF-BD48-70C6B2907D36}"/>
     <cellStyle name="Normal 8" xfId="12" xr:uid="{6299AA32-8A9F-43A0-9B69-D10D8C0FA74E}"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="8">
     <dxf>
       <fill>
         <patternFill>
@@ -887,40 +913,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FF92D050"/>
@@ -1286,19 +1278,19 @@
   <dimension ref="A1:AE51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" customWidth="1"/>
-    <col min="4" max="4" width="23.44140625" customWidth="1"/>
-    <col min="5" max="5" width="72.6640625" customWidth="1"/>
-    <col min="6" max="6" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.125" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="5" max="5" width="72.625" customWidth="1"/>
+    <col min="6" max="6" width="32.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="15" customHeight="1">
+    <row r="1" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1331,7 +1323,7 @@
       <c r="AD1" s="2"/>
       <c r="AE1" s="2"/>
     </row>
-    <row r="2" spans="1:31" ht="15" thickBot="1">
+    <row r="2" spans="1:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1364,7 +1356,7 @@
       <c r="AD2" s="2"/>
       <c r="AE2" s="2"/>
     </row>
-    <row r="3" spans="1:31">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="38" t="s">
         <v>0</v>
@@ -1399,7 +1391,7 @@
       <c r="AD3" s="2"/>
       <c r="AE3" s="2"/>
     </row>
-    <row r="4" spans="1:31" ht="15" thickBot="1">
+    <row r="4" spans="1:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="5" t="s">
         <v>1</v>
@@ -1440,7 +1432,7 @@
       <c r="AD4" s="2"/>
       <c r="AE4" s="2"/>
     </row>
-    <row r="5" spans="1:31">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="8">
         <v>1</v>
@@ -1475,7 +1467,7 @@
       <c r="AD5" s="2"/>
       <c r="AE5" s="2"/>
     </row>
-    <row r="6" spans="1:31">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="13"/>
       <c r="C6" s="25"/>
@@ -1508,7 +1500,7 @@
       <c r="AD6" s="2"/>
       <c r="AE6" s="2"/>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="8"/>
       <c r="C7" s="9"/>
@@ -1541,7 +1533,7 @@
       <c r="AD7" s="2"/>
       <c r="AE7" s="2"/>
     </row>
-    <row r="8" spans="1:31">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="13"/>
       <c r="C8" s="25"/>
@@ -1574,7 +1566,7 @@
       <c r="AD8" s="2"/>
       <c r="AE8" s="2"/>
     </row>
-    <row r="9" spans="1:31">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="8"/>
       <c r="C9" s="9"/>
@@ -1607,7 +1599,7 @@
       <c r="AD9" s="2"/>
       <c r="AE9" s="2"/>
     </row>
-    <row r="10" spans="1:31">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="13"/>
       <c r="C10" s="14"/>
@@ -1640,7 +1632,7 @@
       <c r="AD10" s="2"/>
       <c r="AE10" s="2"/>
     </row>
-    <row r="11" spans="1:31">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="8"/>
       <c r="C11" s="10"/>
@@ -1673,7 +1665,7 @@
       <c r="AD11" s="2"/>
       <c r="AE11" s="2"/>
     </row>
-    <row r="12" spans="1:31">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="13"/>
       <c r="C12" s="14"/>
@@ -1706,7 +1698,7 @@
       <c r="AD12" s="2"/>
       <c r="AE12" s="2"/>
     </row>
-    <row r="13" spans="1:31">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="8"/>
       <c r="C13" s="10"/>
@@ -1739,7 +1731,7 @@
       <c r="AD13" s="2"/>
       <c r="AE13" s="2"/>
     </row>
-    <row r="14" spans="1:31">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" s="13"/>
       <c r="C14" s="14"/>
@@ -1772,7 +1764,7 @@
       <c r="AD14" s="2"/>
       <c r="AE14" s="2"/>
     </row>
-    <row r="15" spans="1:31">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="8"/>
       <c r="C15" s="10"/>
@@ -1805,7 +1797,7 @@
       <c r="AD15" s="2"/>
       <c r="AE15" s="2"/>
     </row>
-    <row r="16" spans="1:31" ht="15" thickBot="1">
+    <row r="16" spans="1:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2"/>
       <c r="B16" s="17"/>
       <c r="C16" s="18"/>
@@ -1838,7 +1830,7 @@
       <c r="AD16" s="2"/>
       <c r="AE16" s="2"/>
     </row>
-    <row r="17" spans="1:31">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1871,7 +1863,7 @@
       <c r="AD17" s="2"/>
       <c r="AE17" s="2"/>
     </row>
-    <row r="18" spans="1:31">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1904,7 +1896,7 @@
       <c r="AD18" s="2"/>
       <c r="AE18" s="2"/>
     </row>
-    <row r="19" spans="1:31">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1937,7 +1929,7 @@
       <c r="AD19" s="2"/>
       <c r="AE19" s="2"/>
     </row>
-    <row r="20" spans="1:31">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1970,7 +1962,7 @@
       <c r="AD20" s="2"/>
       <c r="AE20" s="2"/>
     </row>
-    <row r="21" spans="1:31">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2003,7 +1995,7 @@
       <c r="AD21" s="2"/>
       <c r="AE21" s="2"/>
     </row>
-    <row r="22" spans="1:31">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -2036,7 +2028,7 @@
       <c r="AD22" s="2"/>
       <c r="AE22" s="2"/>
     </row>
-    <row r="23" spans="1:31">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2069,7 +2061,7 @@
       <c r="AD23" s="2"/>
       <c r="AE23" s="2"/>
     </row>
-    <row r="24" spans="1:31">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2102,7 +2094,7 @@
       <c r="AD24" s="2"/>
       <c r="AE24" s="2"/>
     </row>
-    <row r="25" spans="1:31">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2135,7 +2127,7 @@
       <c r="AD25" s="2"/>
       <c r="AE25" s="2"/>
     </row>
-    <row r="26" spans="1:31">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2168,7 +2160,7 @@
       <c r="AD26" s="2"/>
       <c r="AE26" s="2"/>
     </row>
-    <row r="27" spans="1:31">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2201,7 +2193,7 @@
       <c r="AD27" s="2"/>
       <c r="AE27" s="2"/>
     </row>
-    <row r="28" spans="1:31">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2234,7 +2226,7 @@
       <c r="AD28" s="2"/>
       <c r="AE28" s="2"/>
     </row>
-    <row r="29" spans="1:31">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2267,7 +2259,7 @@
       <c r="AD29" s="2"/>
       <c r="AE29" s="2"/>
     </row>
-    <row r="30" spans="1:31">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2300,7 +2292,7 @@
       <c r="AD30" s="2"/>
       <c r="AE30" s="2"/>
     </row>
-    <row r="31" spans="1:31">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2333,7 +2325,7 @@
       <c r="AD31" s="2"/>
       <c r="AE31" s="2"/>
     </row>
-    <row r="32" spans="1:31">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -2366,7 +2358,7 @@
       <c r="AD32" s="2"/>
       <c r="AE32" s="2"/>
     </row>
-    <row r="33" spans="1:31">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -2399,7 +2391,7 @@
       <c r="AD33" s="2"/>
       <c r="AE33" s="2"/>
     </row>
-    <row r="34" spans="1:31">
+    <row r="34" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -2432,7 +2424,7 @@
       <c r="AD34" s="2"/>
       <c r="AE34" s="2"/>
     </row>
-    <row r="35" spans="1:31">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -2465,7 +2457,7 @@
       <c r="AD35" s="2"/>
       <c r="AE35" s="2"/>
     </row>
-    <row r="36" spans="1:31">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -2498,7 +2490,7 @@
       <c r="AD36" s="2"/>
       <c r="AE36" s="2"/>
     </row>
-    <row r="37" spans="1:31">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -2531,7 +2523,7 @@
       <c r="AD37" s="2"/>
       <c r="AE37" s="2"/>
     </row>
-    <row r="38" spans="1:31">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -2564,7 +2556,7 @@
       <c r="AD38" s="2"/>
       <c r="AE38" s="2"/>
     </row>
-    <row r="39" spans="1:31">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2597,7 +2589,7 @@
       <c r="AD39" s="2"/>
       <c r="AE39" s="2"/>
     </row>
-    <row r="40" spans="1:31">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -2630,7 +2622,7 @@
       <c r="AD40" s="2"/>
       <c r="AE40" s="2"/>
     </row>
-    <row r="41" spans="1:31">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2663,7 +2655,7 @@
       <c r="AD41" s="2"/>
       <c r="AE41" s="2"/>
     </row>
-    <row r="42" spans="1:31">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2696,7 +2688,7 @@
       <c r="AD42" s="2"/>
       <c r="AE42" s="2"/>
     </row>
-    <row r="43" spans="1:31">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2729,7 +2721,7 @@
       <c r="AD43" s="2"/>
       <c r="AE43" s="2"/>
     </row>
-    <row r="44" spans="1:31">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2762,7 +2754,7 @@
       <c r="AD44" s="2"/>
       <c r="AE44" s="2"/>
     </row>
-    <row r="45" spans="1:31">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2795,7 +2787,7 @@
       <c r="AD45" s="2"/>
       <c r="AE45" s="2"/>
     </row>
-    <row r="46" spans="1:31">
+    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2828,7 +2820,7 @@
       <c r="AD46" s="2"/>
       <c r="AE46" s="2"/>
     </row>
-    <row r="47" spans="1:31">
+    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2861,7 +2853,7 @@
       <c r="AD47" s="2"/>
       <c r="AE47" s="2"/>
     </row>
-    <row r="48" spans="1:31">
+    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2894,7 +2886,7 @@
       <c r="AD48" s="2"/>
       <c r="AE48" s="2"/>
     </row>
-    <row r="49" spans="1:31">
+    <row r="49" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -2927,7 +2919,7 @@
       <c r="AD49" s="2"/>
       <c r="AE49" s="2"/>
     </row>
-    <row r="50" spans="1:31">
+    <row r="50" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2960,7 +2952,7 @@
       <c r="AD50" s="2"/>
       <c r="AE50" s="2"/>
     </row>
-    <row r="51" spans="1:31">
+    <row r="51" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -3011,43 +3003,44 @@
       <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T15" sqref="T15"/>
+      <selection pane="bottomRight" activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultRowHeight="16.5" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="17.5546875" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="30.33203125" hidden="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.5546875" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5546875" style="27" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="27.44140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="17.5" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="30.375" hidden="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="16.5" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="23.5" style="27" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="27.5" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="22" style="28" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="11" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5546875" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="6.6640625" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="5.88671875" style="29" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="27.33203125" style="27" customWidth="1"/>
-    <col min="17" max="17" width="20.44140625" style="27" customWidth="1"/>
-    <col min="18" max="18" width="13.5546875" style="27" customWidth="1"/>
-    <col min="19" max="19" width="24.88671875" customWidth="1"/>
-    <col min="20" max="20" width="49.33203125" customWidth="1"/>
-    <col min="21" max="21" width="27.88671875" style="29" customWidth="1"/>
-    <col min="22" max="22" width="14.44140625" customWidth="1"/>
-    <col min="23" max="23" width="25.6640625" customWidth="1"/>
-    <col min="24" max="24" width="15.6640625" customWidth="1"/>
-    <col min="25" max="25" width="19.77734375" customWidth="1"/>
-    <col min="26" max="26" width="93.5546875" customWidth="1"/>
+    <col min="11" max="11" width="8.5" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="6.625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="5.875" style="29" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="33.5" style="27" customWidth="1"/>
+    <col min="15" max="16" width="27.375" style="27" customWidth="1"/>
+    <col min="17" max="17" width="20.5" style="27" customWidth="1"/>
+    <col min="18" max="18" width="13.5" style="27" customWidth="1"/>
+    <col min="19" max="19" width="24.875" customWidth="1"/>
+    <col min="20" max="20" width="49.375" customWidth="1"/>
+    <col min="21" max="21" width="27.875" style="29" customWidth="1"/>
+    <col min="22" max="22" width="14.5" customWidth="1"/>
+    <col min="23" max="23" width="25.625" customWidth="1"/>
+    <col min="24" max="24" width="15.625" customWidth="1"/>
+    <col min="25" max="25" width="19.75" customWidth="1"/>
+    <col min="26" max="26" width="93.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="13:22">
+    <row r="1" spans="13:22" x14ac:dyDescent="0.3">
       <c r="M1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="O1" s="26" t="s">
         <v>8</v>
@@ -3055,122 +3048,122 @@
       <c r="P1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" s="41" t="s">
+      <c r="Q1" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="50"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="42"/>
-      <c r="S1" s="43"/>
-      <c r="T1" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="U1" s="42"/>
-      <c r="V1" s="43"/>
-    </row>
-    <row r="2" spans="13:22" ht="24.6" customHeight="1">
-      <c r="M2" s="48">
+      <c r="U1" s="50"/>
+      <c r="V1" s="51"/>
+    </row>
+    <row r="2" spans="13:22" ht="24.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M2" s="43">
         <v>1</v>
       </c>
-      <c r="N2" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2" s="46" t="s">
+      <c r="N2" s="41" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="P2" s="54" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q2" s="44" t="s">
+      <c r="P2" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="R2" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="R2" s="34" t="s">
-        <v>28</v>
-      </c>
       <c r="S2" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="T2" s="44" t="s">
-        <v>26</v>
+        <v>31</v>
+      </c>
+      <c r="T2" s="41" t="s">
+        <v>37</v>
       </c>
       <c r="U2" s="34" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="V2" s="36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="13:22" ht="125.4" customHeight="1">
-      <c r="M3" s="49"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="55"/>
-      <c r="Q3" s="45"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="13:22" ht="125.45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M3" s="44"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="42"/>
       <c r="R3" s="34" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="S3" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="T3" s="45"/>
+      <c r="T3" s="42"/>
       <c r="U3" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="V3" s="37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="13:22" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="M4" s="43">
+        <v>2</v>
+      </c>
+      <c r="N4" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="P4" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="41" t="s">
+        <v>21</v>
+      </c>
+      <c r="R4" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="S4" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="T4" s="41" t="s">
+        <v>22</v>
+      </c>
+      <c r="U4" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="V4" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="V3" s="37" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="13:22" ht="43.2">
-      <c r="M4" s="48">
-        <v>2</v>
-      </c>
-      <c r="N4" s="44" t="s">
+    </row>
+    <row r="5" spans="13:22" ht="132" x14ac:dyDescent="0.3">
+      <c r="M5" s="44"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="34" t="s">
         <v>23</v>
-      </c>
-      <c r="O4" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="P4" s="54" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q4" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="R4" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="S4" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="T4" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="U4" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="V4" s="36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="13:22" ht="115.2">
-      <c r="M5" s="49"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="47"/>
-      <c r="P5" s="55"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="34" t="s">
-        <v>27</v>
       </c>
       <c r="S5" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="T5" s="45"/>
+      <c r="T5" s="42"/>
       <c r="U5" s="34" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="V5" s="37" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="13:22">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="13:22" x14ac:dyDescent="0.3">
       <c r="M6" s="35"/>
       <c r="N6" s="35"/>
       <c r="O6" s="35"/>
@@ -3179,7 +3172,7 @@
       <c r="R6"/>
       <c r="U6"/>
     </row>
-    <row r="7" spans="13:22">
+    <row r="7" spans="13:22" x14ac:dyDescent="0.3">
       <c r="M7" s="35"/>
       <c r="N7" s="35"/>
       <c r="O7" s="35"/>
@@ -3188,7 +3181,7 @@
       <c r="R7"/>
       <c r="U7"/>
     </row>
-    <row r="8" spans="13:22">
+    <row r="8" spans="13:22" x14ac:dyDescent="0.3">
       <c r="M8" s="35"/>
       <c r="N8" s="35"/>
       <c r="O8" s="35"/>
@@ -3197,7 +3190,7 @@
       <c r="R8"/>
       <c r="U8"/>
     </row>
-    <row r="9" spans="13:22">
+    <row r="9" spans="13:22" x14ac:dyDescent="0.3">
       <c r="M9" s="35"/>
       <c r="N9" s="35"/>
       <c r="O9" s="35"/>
@@ -3206,7 +3199,7 @@
       <c r="R9"/>
       <c r="U9"/>
     </row>
-    <row r="10" spans="13:22">
+    <row r="10" spans="13:22" x14ac:dyDescent="0.3">
       <c r="M10" s="35"/>
       <c r="N10" s="35"/>
       <c r="O10" s="35"/>
@@ -3215,16 +3208,18 @@
       <c r="R10"/>
       <c r="U10"/>
     </row>
-    <row r="11" spans="13:22">
+    <row r="11" spans="13:22" x14ac:dyDescent="0.3">
       <c r="M11" s="35"/>
       <c r="N11" s="35"/>
-      <c r="O11" s="35"/>
+      <c r="O11" s="35" t="s">
+        <v>38</v>
+      </c>
       <c r="P11" s="35"/>
       <c r="Q11"/>
       <c r="R11"/>
       <c r="U11"/>
     </row>
-    <row r="12" spans="13:22">
+    <row r="12" spans="13:22" x14ac:dyDescent="0.3">
       <c r="M12" s="35"/>
       <c r="N12" s="35"/>
       <c r="O12" s="35"/>
@@ -3233,7 +3228,7 @@
       <c r="R12"/>
       <c r="U12"/>
     </row>
-    <row r="13" spans="13:22">
+    <row r="13" spans="13:22" x14ac:dyDescent="0.3">
       <c r="M13" s="35"/>
       <c r="N13" s="35"/>
       <c r="O13" s="35"/>
@@ -3242,7 +3237,7 @@
       <c r="R13"/>
       <c r="U13"/>
     </row>
-    <row r="14" spans="13:22">
+    <row r="14" spans="13:22" x14ac:dyDescent="0.3">
       <c r="M14" s="35"/>
       <c r="N14" s="35"/>
       <c r="O14" s="35"/>
@@ -3251,7 +3246,7 @@
       <c r="R14"/>
       <c r="U14"/>
     </row>
-    <row r="15" spans="13:22">
+    <row r="15" spans="13:22" x14ac:dyDescent="0.3">
       <c r="M15" s="35"/>
       <c r="N15" s="35"/>
       <c r="O15" s="35"/>
@@ -3260,7 +3255,7 @@
       <c r="R15"/>
       <c r="U15"/>
     </row>
-    <row r="16" spans="13:22">
+    <row r="16" spans="13:22" x14ac:dyDescent="0.3">
       <c r="M16" s="35"/>
       <c r="N16" s="35"/>
       <c r="O16" s="35"/>
@@ -3269,7 +3264,7 @@
       <c r="R16"/>
       <c r="U16"/>
     </row>
-    <row r="17" spans="13:21">
+    <row r="17" spans="13:21" x14ac:dyDescent="0.3">
       <c r="M17" s="35"/>
       <c r="N17" s="35"/>
       <c r="O17" s="35"/>
@@ -3279,7 +3274,7 @@
       <c r="S17" s="29"/>
       <c r="U17"/>
     </row>
-    <row r="18" spans="13:21">
+    <row r="18" spans="13:21" x14ac:dyDescent="0.3">
       <c r="M18" s="35"/>
       <c r="N18" s="35"/>
       <c r="O18" s="35"/>
@@ -3289,7 +3284,7 @@
       <c r="S18" s="29"/>
       <c r="U18"/>
     </row>
-    <row r="19" spans="13:21">
+    <row r="19" spans="13:21" x14ac:dyDescent="0.3">
       <c r="M19" s="35"/>
       <c r="N19" s="35"/>
       <c r="O19" s="35"/>
@@ -3299,7 +3294,7 @@
       <c r="S19" s="29"/>
       <c r="U19"/>
     </row>
-    <row r="20" spans="13:21">
+    <row r="20" spans="13:21" x14ac:dyDescent="0.3">
       <c r="M20" s="27"/>
       <c r="Q20"/>
       <c r="R20"/>
@@ -3308,12 +3303,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="T4:T5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="O4:O5"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="T1:V1"/>
     <mergeCell ref="T2:T3"/>
     <mergeCell ref="O2:O3"/>
@@ -3322,6 +3311,12 @@
     <mergeCell ref="Q1:S1"/>
     <mergeCell ref="Q2:Q3"/>
     <mergeCell ref="P2:P3"/>
+    <mergeCell ref="T4:T5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="P2">
@@ -3355,48 +3350,48 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" customWidth="1"/>
-    <col min="2" max="2" width="35.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.875" customWidth="1"/>
+    <col min="2" max="2" width="35.625" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="37.88671875" customWidth="1"/>
-    <col min="5" max="5" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.875" customWidth="1"/>
+    <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="4.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="52" t="s">
+      <c r="B1" s="52"/>
+      <c r="C1" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-    </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
       <c r="C2" s="21" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
@@ -3406,7 +3401,7 @@
       <c r="J2" s="22"/>
       <c r="K2" s="22"/>
     </row>
-    <row r="3" spans="1:11" ht="16.5" customHeight="1">
+    <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33" t="s">
         <v>14</v>
       </c>
@@ -3427,7 +3422,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -3464,31 +3459,31 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" customWidth="1"/>
-    <col min="2" max="2" width="49.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.875" customWidth="1"/>
+    <col min="2" max="2" width="49.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="52" t="s">
+      <c r="B1" s="52"/>
+      <c r="C1" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="50"/>
-      <c r="B2" s="50"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="52"/>
+      <c r="B2" s="52"/>
       <c r="C2" s="21" t="s">
         <v>8</v>
       </c>
@@ -3496,7 +3491,7 @@
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
     </row>
-    <row r="3" spans="1:6" ht="16.5" customHeight="1">
+    <row r="3" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33"/>
       <c r="B3" s="23"/>
       <c r="C3" s="1"/>
@@ -3504,7 +3499,7 @@
       <c r="E3" s="30"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -3534,18 +3529,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3760,14 +3755,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFD46AAD-E98A-4FA8-BFA3-1BCF67823CB2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96EC4C15-7EED-4784-8F5D-530E01EF32B0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="ce510894-e256-4a70-bf8c-71462871c739"/>
@@ -3780,6 +3767,14 @@
     <ds:schemaRef ds:uri="b0add36e-da03-4abd-a3e0-9f2a80588293"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFD46AAD-E98A-4FA8-BFA3-1BCF67823CB2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>